<commit_message>
note: add more test cases
</commit_message>
<xml_diff>
--- a/tests/input/header_image10.xlsx
+++ b/tests/input/header_image10.xlsx
@@ -384,8 +384,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G</oddHeader>
   </headerFooter>
@@ -409,7 +409,7 @@
     <row r="2" spans="1:2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>